<commit_message>
atualizado todo o treinamento para o novo lm
</commit_message>
<xml_diff>
--- a/fuction_ensemble_2/redes-ensemble-s/Teste01/content/results/metrics_10_1.xlsx
+++ b/fuction_ensemble_2/redes-ensemble-s/Teste01/content/results/metrics_10_1.xlsx
@@ -518,56 +518,56 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_10</t>
+          <t>model_10_1_8</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9998683818693125</v>
+        <v>0.999859555414342</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9993432993160948</v>
+        <v>0.9992044290983603</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9994882995524171</v>
+        <v>0.9998187217291216</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9998559304683906</v>
+        <v>0.9999217089966091</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9996293501934409</v>
+        <v>0.9998832266752921</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0001228597476285432</v>
+        <v>0.0001310988559069337</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0006130012625970681</v>
+        <v>0.0007426305151541182</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0002628636722470595</v>
+        <v>0.0001402973658467337</v>
       </c>
       <c r="J2" t="n">
-        <v>3.691450176380139e-05</v>
+        <v>0.0001014588894934918</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0001498890870054304</v>
+        <v>0.0001208781276701127</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0009756343721635678</v>
+        <v>0.001293170784412817</v>
       </c>
       <c r="M2" t="n">
-        <v>0.01108421163766477</v>
+        <v>0.01144984086819261</v>
       </c>
       <c r="N2" t="n">
-        <v>1.0006317670273</v>
+        <v>1.000674134011158</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0115560894745614</v>
+        <v>0.01193728429838965</v>
       </c>
       <c r="P2" t="n">
-        <v>76.00893423273821</v>
+        <v>75.87911778821164</v>
       </c>
       <c r="Q2" t="n">
-        <v>111.356333153916</v>
+        <v>111.2265167093895</v>
       </c>
     </row>
     <row r="3">
@@ -577,1097 +577,1097 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9998481616902142</v>
+        <v>0.9998754697602077</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9993426773716413</v>
+        <v>0.9992035975555886</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9994817077049096</v>
+        <v>0.9997954415776454</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9998547448651991</v>
+        <v>0.9999492532751921</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9996247877578229</v>
+        <v>0.9998917654665056</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0001417343972535572</v>
+        <v>0.0001162435126003626</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0006135818204441462</v>
+        <v>0.0007434067238309347</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0002662499449206196</v>
+        <v>0.0001583146599922303</v>
       </c>
       <c r="J3" t="n">
-        <v>3.721828529537213e-05</v>
+        <v>6.576370363702477e-05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0001517341151079959</v>
+        <v>0.0001120391818146275</v>
       </c>
       <c r="L3" t="n">
-        <v>0.001055507724153886</v>
+        <v>0.001214732167363087</v>
       </c>
       <c r="M3" t="n">
-        <v>0.01190522562799871</v>
+        <v>0.01078162847627216</v>
       </c>
       <c r="N3" t="n">
-        <v>1.000728823886972</v>
+        <v>1.000597745151003</v>
       </c>
       <c r="O3" t="n">
-        <v>0.0124120557301971</v>
+        <v>0.0112406247215548</v>
       </c>
       <c r="P3" t="n">
-        <v>75.72311138740025</v>
+        <v>76.11964664128456</v>
       </c>
       <c r="Q3" t="n">
-        <v>111.0705103085781</v>
+        <v>111.4670455624624</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_11</t>
+          <t>model_10_1_7</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9998854069089282</v>
+        <v>0.9998378864660934</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9993413539636842</v>
+        <v>0.9991968962271144</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9995009340057529</v>
+        <v>0.9998350756910723</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9998561066727583</v>
+        <v>0.9998836692290487</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9996374308298444</v>
+        <v>0.9998655289734235</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001069676204601478</v>
+        <v>0.0001513258679401176</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0006148171636811772</v>
+        <v>0.0007496621198073834</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0002563732757340532</v>
+        <v>0.0001276404832996097</v>
       </c>
       <c r="J4" t="n">
-        <v>3.686935344987827e-05</v>
+        <v>0.000150755391085154</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0001466213145919657</v>
+        <v>0.0001391979371923819</v>
       </c>
       <c r="L4" t="n">
-        <v>0.000901942367393936</v>
+        <v>0.001364869827179656</v>
       </c>
       <c r="M4" t="n">
-        <v>0.01034251519023046</v>
+        <v>0.01230145795993782</v>
       </c>
       <c r="N4" t="n">
-        <v>1.000550046837144</v>
+        <v>1.000778144962752</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0107828174738365</v>
+        <v>0.01282515649282087</v>
       </c>
       <c r="P4" t="n">
-        <v>76.28596876364152</v>
+        <v>75.59214996120002</v>
       </c>
       <c r="Q4" t="n">
-        <v>111.6333676848193</v>
+        <v>110.9395488823778</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_12</t>
+          <t>model_10_1_10</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9998990566963925</v>
+        <v>0.999886545985384</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9993382699087517</v>
+        <v>0.9991918733665495</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9995120634156507</v>
+        <v>0.999791056336281</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9998553609792608</v>
+        <v>0.9999623376703729</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9996442634734072</v>
+        <v>0.9998983164110909</v>
       </c>
       <c r="G5" t="n">
-        <v>9.422614301875412e-05</v>
+        <v>0.0001059043425883672</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0006176959935862863</v>
+        <v>0.0007543507396666126</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0002506560293069997</v>
+        <v>0.0001617085461378515</v>
       </c>
       <c r="J5" t="n">
-        <v>3.70604202467438e-05</v>
+        <v>4.880737216535951e-05</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0001438582247768717</v>
+        <v>0.0001052579591516055</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0008368302942237427</v>
+        <v>0.00115598642950934</v>
       </c>
       <c r="M5" t="n">
-        <v>0.00970701514466492</v>
+        <v>0.0102909835578708</v>
       </c>
       <c r="N5" t="n">
-        <v>1.000484527857316</v>
+        <v>1.000544579270157</v>
       </c>
       <c r="O5" t="n">
-        <v>0.01012026287566478</v>
+        <v>0.0107290920332021</v>
       </c>
       <c r="P5" t="n">
-        <v>76.53962577629403</v>
+        <v>76.30594859939498</v>
       </c>
       <c r="Q5" t="n">
-        <v>111.8870246974718</v>
+        <v>111.6533475205728</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_8</t>
+          <t>model_10_1_11</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9998239829558143</v>
+        <v>0.9998952392633419</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9993379722084854</v>
+        <v>0.9991889481948873</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9994819648735487</v>
+        <v>0.9997538984147776</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9998537482593749</v>
+        <v>0.9999757911686477</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9996246353720843</v>
+        <v>0.9998928471129218</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0001643041844920057</v>
+        <v>9.778954920549156e-05</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0006179738837173541</v>
+        <v>0.0007570812590130359</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0002661178358064652</v>
+        <v>0.0001904663144131361</v>
       </c>
       <c r="J6" t="n">
-        <v>3.747364260130232e-05</v>
+        <v>3.13727125538989e-05</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0001517957392038837</v>
+        <v>0.0001109195134835175</v>
       </c>
       <c r="L6" t="n">
-        <v>0.001141896593695045</v>
+        <v>0.001075058836305462</v>
       </c>
       <c r="M6" t="n">
-        <v>0.01281811938203127</v>
+        <v>0.009888859853668245</v>
       </c>
       <c r="N6" t="n">
-        <v>1.000844881812091</v>
+        <v>1.000502851535959</v>
       </c>
       <c r="O6" t="n">
-        <v>0.01336381326128942</v>
+        <v>0.01030984909040082</v>
       </c>
       <c r="P6" t="n">
-        <v>75.42758212927825</v>
+        <v>76.46538569094574</v>
       </c>
       <c r="Q6" t="n">
-        <v>110.7749810504561</v>
+        <v>111.8127846121236</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_13</t>
+          <t>model_10_1_12</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9999095833600844</v>
+        <v>0.999900825465485</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9993351438205954</v>
+        <v>0.9991824909920624</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9995176114321227</v>
+        <v>0.9997177159234797</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9998530016786664</v>
+        <v>0.999982044328563</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9996470398818532</v>
+        <v>0.9998832353573067</v>
       </c>
       <c r="G7" t="n">
-        <v>8.439996452946082e-05</v>
+        <v>9.25750747108727e-05</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0006206140596607893</v>
+        <v>0.0007631087744117284</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0002478059790668532</v>
+        <v>0.0002184691643645614</v>
       </c>
       <c r="J7" t="n">
-        <v>3.766493672554407e-05</v>
+        <v>2.32691165678127e-05</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0001427354578961987</v>
+        <v>0.000120869140466187</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0007801293020040684</v>
+        <v>0.001017366216656822</v>
       </c>
       <c r="M7" t="n">
-        <v>0.009186945331798858</v>
+        <v>0.009621594187600759</v>
       </c>
       <c r="N7" t="n">
-        <v>1.000433999871595</v>
+        <v>1.000476037765672</v>
       </c>
       <c r="O7" t="n">
-        <v>0.009578052614172085</v>
+        <v>0.01003120537161264</v>
       </c>
       <c r="P7" t="n">
-        <v>76.759887153259</v>
+        <v>76.57498124826833</v>
       </c>
       <c r="Q7" t="n">
-        <v>112.1072860744368</v>
+        <v>111.9223801694461</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_14</t>
+          <t>model_10_1_13</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9999176339049701</v>
+        <v>0.9999050472647075</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9993319848622311</v>
+        <v>0.9991731062127861</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9995187043869425</v>
+        <v>0.9996876865052019</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9998497586527998</v>
+        <v>0.9999833216339492</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9996467066769025</v>
+        <v>0.9998728091127567</v>
       </c>
       <c r="G8" t="n">
-        <v>7.688513425667218e-05</v>
+        <v>8.863421045212147e-05</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0006235628086316699</v>
+        <v>0.0007718690539218417</v>
       </c>
       <c r="I8" t="n">
-        <v>0.0002472445214428063</v>
+        <v>0.0002417099436475295</v>
       </c>
       <c r="J8" t="n">
-        <v>3.849588746671892e-05</v>
+        <v>2.161383076968722e-05</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0001428702044547626</v>
+        <v>0.0001316618872086084</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0007306234515267343</v>
+        <v>0.0009672008361185586</v>
       </c>
       <c r="M8" t="n">
-        <v>0.008768416861479169</v>
+        <v>0.009414574363831935</v>
       </c>
       <c r="N8" t="n">
-        <v>1.000395357256143</v>
+        <v>1.000455773129404</v>
       </c>
       <c r="O8" t="n">
-        <v>0.009141706520397516</v>
+        <v>0.009815372285355867</v>
       </c>
       <c r="P8" t="n">
-        <v>76.94639602559407</v>
+        <v>76.66198530478979</v>
       </c>
       <c r="Q8" t="n">
-        <v>112.2937949467719</v>
+        <v>112.0093842259676</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_15</t>
+          <t>model_10_1_6</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.999923946076073</v>
+        <v>0.9998082049654381</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9993285582660327</v>
+        <v>0.9991723120325228</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9995192014891994</v>
+        <v>0.9998393416652641</v>
       </c>
       <c r="E9" t="n">
-        <v>0.999845554363715</v>
+        <v>0.9998294395393016</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9996456904836298</v>
+        <v>0.999833178278054</v>
       </c>
       <c r="G9" t="n">
-        <v>7.099299960441958e-05</v>
+        <v>0.00017903224593449</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0006267613857726484</v>
+        <v>0.000772610386337183</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0002469891569510416</v>
+        <v>0.000124338902040157</v>
       </c>
       <c r="J9" t="n">
-        <v>3.95731397844076e-05</v>
+        <v>0.0002210327391968107</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0001432811483677246</v>
+        <v>0.0001726858206184838</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0006869521164321691</v>
+        <v>0.001456289950113991</v>
       </c>
       <c r="M9" t="n">
-        <v>0.008425734365882868</v>
+        <v>0.01338029319314379</v>
       </c>
       <c r="N9" t="n">
-        <v>1.000365058834849</v>
+        <v>1.000920616165897</v>
       </c>
       <c r="O9" t="n">
-        <v>0.008784435321513124</v>
+        <v>0.01394991997540121</v>
       </c>
       <c r="P9" t="n">
-        <v>77.10585856580965</v>
+        <v>75.25588924692448</v>
       </c>
       <c r="Q9" t="n">
-        <v>112.4532574869875</v>
+        <v>110.6032881681023</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_7</t>
+          <t>model_10_1_14</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9997951647880767</v>
+        <v>0.9999089660754459</v>
       </c>
       <c r="C10" t="n">
-        <v>0.9993277367894744</v>
+        <v>0.999164662719223</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9994913398301484</v>
+        <v>0.9996595629989277</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9998524813718743</v>
+        <v>0.999980802241896</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9996301885533128</v>
+        <v>0.9998607187804419</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0001912046791037461</v>
+        <v>8.49761726437732e-05</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0006275281980812067</v>
+        <v>0.0007797506845365205</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0002613018628469025</v>
+        <v>0.0002634756733708806</v>
       </c>
       <c r="J10" t="n">
-        <v>3.779825336633206e-05</v>
+        <v>2.487876171765172e-05</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0001495500581066173</v>
+        <v>0.0001441772175442662</v>
       </c>
       <c r="L10" t="n">
-        <v>0.001234619881336541</v>
+        <v>0.0009097930663482078</v>
       </c>
       <c r="M10" t="n">
-        <v>0.01382767800839122</v>
+        <v>0.00921825214689711</v>
       </c>
       <c r="N10" t="n">
-        <v>1.000983209017232</v>
+        <v>1.00043696283786</v>
       </c>
       <c r="O10" t="n">
-        <v>0.01441635088844797</v>
+        <v>0.009610692225203112</v>
       </c>
       <c r="P10" t="n">
-        <v>75.12433217069298</v>
+        <v>76.74627932521886</v>
       </c>
       <c r="Q10" t="n">
-        <v>110.4717310918708</v>
+        <v>112.0936782463967</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_16</t>
+          <t>model_10_1_15</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9999289394532158</v>
+        <v>0.9999106698842326</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9993249452395796</v>
+        <v>0.9991510847985495</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9995191146235415</v>
+        <v>0.99962815112359</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9998408715606858</v>
+        <v>0.9999757615857152</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9996441517867977</v>
+        <v>0.999845820968009</v>
       </c>
       <c r="G11" t="n">
-        <v>6.633190122557797e-05</v>
+        <v>8.338574192998051e-05</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0006301339873731344</v>
+        <v>0.0007924250774833854</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0002470337803746226</v>
+        <v>0.000287786382783599</v>
       </c>
       <c r="J11" t="n">
-        <v>4.077300028754889e-05</v>
+        <v>3.141104967240957e-05</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0001439033903310858</v>
+        <v>0.0001595987162280043</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0006478042211701222</v>
+        <v>0.0008592307619943073</v>
       </c>
       <c r="M11" t="n">
-        <v>0.008144439896369668</v>
+        <v>0.00913157937763126</v>
       </c>
       <c r="N11" t="n">
-        <v>1.000341090624564</v>
+        <v>1.000428784555683</v>
       </c>
       <c r="O11" t="n">
-        <v>0.00849116556407292</v>
+        <v>0.009520329616712248</v>
       </c>
       <c r="P11" t="n">
-        <v>77.2416792234102</v>
+        <v>76.78406644657417</v>
       </c>
       <c r="Q11" t="n">
-        <v>112.589078144588</v>
+        <v>112.131465367752</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_17</t>
+          <t>model_10_1_16</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9999328045141779</v>
+        <v>0.9999102481505852</v>
       </c>
       <c r="C12" t="n">
-        <v>0.999321495089133</v>
+        <v>0.999138377136956</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9995180401242298</v>
+        <v>0.9995894030996948</v>
       </c>
       <c r="E12" t="n">
-        <v>0.999835847108444</v>
+        <v>0.9999693079106708</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9996418775558825</v>
+        <v>0.9998272962229374</v>
       </c>
       <c r="G12" t="n">
-        <v>6.272403647399133e-05</v>
+        <v>8.377941177784731e-05</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0006333545513708483</v>
+        <v>0.0008042871217790723</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0002475857572904481</v>
+        <v>0.0003177747849121487</v>
       </c>
       <c r="J12" t="n">
-        <v>4.206040053845502e-05</v>
+        <v>3.977449725633933e-05</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0001448230789144516</v>
+        <v>0.000178774641084244</v>
       </c>
       <c r="L12" t="n">
-        <v>0.0006130088171729809</v>
+        <v>0.0008137655556271049</v>
       </c>
       <c r="M12" t="n">
-        <v>0.007919850786093847</v>
+        <v>0.009153109404887899</v>
       </c>
       <c r="N12" t="n">
-        <v>1.000322538331946</v>
+        <v>1.000430808877191</v>
       </c>
       <c r="O12" t="n">
-        <v>0.008257015230409108</v>
+        <v>0.009542776221802503</v>
       </c>
       <c r="P12" t="n">
-        <v>77.35353165389179</v>
+        <v>76.77464652700625</v>
       </c>
       <c r="Q12" t="n">
-        <v>112.7009305750696</v>
+        <v>112.1220454481841</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_18</t>
+          <t>model_10_1_5</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9999358229518556</v>
+        <v>0.9997732874725364</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9993181372075147</v>
+        <v>0.9991352796012597</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9995167458832462</v>
+        <v>0.9998245335622004</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9998306900126079</v>
+        <v>0.9997596869106429</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9996394217334991</v>
+        <v>0.9997839805086902</v>
       </c>
       <c r="G13" t="n">
-        <v>5.990645739598236e-05</v>
+        <v>0.0002116261928574525</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0006364889864675545</v>
+        <v>0.0008071785353854145</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0002482506168568943</v>
+        <v>0.0001357993922741352</v>
       </c>
       <c r="J13" t="n">
-        <v>4.338178765765419e-05</v>
+        <v>0.0003114265767574485</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0001458162022572742</v>
+        <v>0.0002236129845157918</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0005826911093101553</v>
+        <v>0.001582513731860857</v>
       </c>
       <c r="M13" t="n">
-        <v>0.007739926188019003</v>
+        <v>0.01454737752508859</v>
       </c>
       <c r="N13" t="n">
-        <v>1.000308049831093</v>
+        <v>1.001088220131825</v>
       </c>
       <c r="O13" t="n">
-        <v>0.008069430869698952</v>
+        <v>0.01516668950355453</v>
       </c>
       <c r="P13" t="n">
-        <v>77.4454525114305</v>
+        <v>74.92137816174053</v>
       </c>
       <c r="Q13" t="n">
-        <v>112.7928514326083</v>
+        <v>110.2687770829183</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_19</t>
+          <t>model_10_1_17</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9999382424593672</v>
+        <v>0.9999100665109217</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9993148564834659</v>
+        <v>0.9991272966162738</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9995159641858565</v>
+        <v>0.9995620740772677</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9998254621964023</v>
+        <v>0.9999608368705392</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9996372690504662</v>
+        <v>0.9998117774165228</v>
       </c>
       <c r="G14" t="n">
-        <v>5.764795333792316e-05</v>
+        <v>8.394896443067213e-05</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0006395513983600327</v>
+        <v>0.0008146303014572692</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0002486521796216075</v>
+        <v>0.0003389256367992219</v>
       </c>
       <c r="J14" t="n">
-        <v>4.472129524393613e-05</v>
+        <v>5.075228892322401e-05</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0001466867374327718</v>
+        <v>0.000194838962861223</v>
       </c>
       <c r="L14" t="n">
-        <v>0.000555889238165243</v>
+        <v>0.000764353589887182</v>
       </c>
       <c r="M14" t="n">
-        <v>0.007592624930676029</v>
+        <v>0.009162366748317387</v>
       </c>
       <c r="N14" t="n">
-        <v>1.000296436195037</v>
+        <v>1.000431680747576</v>
       </c>
       <c r="O14" t="n">
-        <v>0.00791585869287525</v>
+        <v>0.009552427669507126</v>
       </c>
       <c r="P14" t="n">
-        <v>77.52231162677968</v>
+        <v>76.77060302013136</v>
       </c>
       <c r="Q14" t="n">
-        <v>112.8697105479575</v>
+        <v>112.1180019413092</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_20</t>
+          <t>model_10_1_18</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9999401390322927</v>
+        <v>0.9999094804815305</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9993116565203572</v>
+        <v>0.9991166678091634</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9995152303305187</v>
+        <v>0.9995394987524202</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9998203681464612</v>
+        <v>0.9999519863063576</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9996351891319597</v>
+        <v>0.9997977981010757</v>
       </c>
       <c r="G15" t="n">
-        <v>5.587758576194873e-05</v>
+        <v>8.449599714367644e-05</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0006425384234598583</v>
+        <v>0.0008245518263440045</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0002490291656295491</v>
+        <v>0.000356397441852806</v>
       </c>
       <c r="J15" t="n">
-        <v>4.60265283035025e-05</v>
+        <v>6.22219134568707e-05</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0001475278469665258</v>
+        <v>0.0002093096776548384</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0005328264285946295</v>
+        <v>0.0007266299037035841</v>
       </c>
       <c r="M15" t="n">
-        <v>0.007475131153494815</v>
+        <v>0.009192170426165762</v>
       </c>
       <c r="N15" t="n">
-        <v>1.000287332644995</v>
+        <v>1.000434493688654</v>
       </c>
       <c r="O15" t="n">
-        <v>0.007793362962353784</v>
+        <v>0.009583500151623625</v>
       </c>
       <c r="P15" t="n">
-        <v>77.5846944569651</v>
+        <v>76.75761279160788</v>
       </c>
       <c r="Q15" t="n">
-        <v>112.9320933781429</v>
+        <v>112.1050117127857</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_6</t>
+          <t>model_10_1_19</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9997608465591423</v>
+        <v>0.9999079259952591</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9993100874796305</v>
+        <v>0.9991062988360984</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9995122687454078</v>
+        <v>0.9995165290065438</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9998497782048774</v>
+        <v>0.9999427697697444</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9996426252522522</v>
+        <v>0.9997834422578977</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0002232392394178139</v>
+        <v>8.594704184388985e-05</v>
       </c>
       <c r="H16" t="n">
-        <v>0.0006440030541053842</v>
+        <v>0.0008342308075549692</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0002505505501458298</v>
+        <v>0.0003741745026390427</v>
       </c>
       <c r="J16" t="n">
-        <v>3.849087769681009e-05</v>
+        <v>7.416580904197041e-05</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0001445207139213199</v>
+        <v>0.0002241701558405065</v>
       </c>
       <c r="L16" t="n">
-        <v>0.001333618668249549</v>
+        <v>0.0006945385048055931</v>
       </c>
       <c r="M16" t="n">
-        <v>0.01494119270399167</v>
+        <v>0.009270762743371758</v>
       </c>
       <c r="N16" t="n">
-        <v>1.001147936516117</v>
+        <v>1.000441955222756</v>
       </c>
       <c r="O16" t="n">
-        <v>0.01557727020993332</v>
+        <v>0.009665438306481606</v>
       </c>
       <c r="P16" t="n">
-        <v>74.81453307813111</v>
+        <v>76.72355848780352</v>
       </c>
       <c r="Q16" t="n">
-        <v>110.1619319993089</v>
+        <v>112.0709574089813</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_21</t>
+          <t>model_10_1_20</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9999416253541085</v>
+        <v>0.999905571266723</v>
       </c>
       <c r="C17" t="n">
-        <v>0.999308655246378</v>
+        <v>0.9990961910904718</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9995144788908906</v>
+        <v>0.999493060411345</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9998154504929592</v>
+        <v>0.9999330065409237</v>
       </c>
       <c r="F17" t="n">
-        <v>0.999633153927571</v>
+        <v>0.9997685577262376</v>
       </c>
       <c r="G17" t="n">
-        <v>5.449016958889588e-05</v>
+        <v>8.814507757181329e-05</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0006453399809787578</v>
+        <v>0.000843665944418652</v>
       </c>
       <c r="I17" t="n">
-        <v>0.000249415184795727</v>
+        <v>0.000392337639735091</v>
       </c>
       <c r="J17" t="n">
-        <v>4.728656383529552e-05</v>
+        <v>8.681817407906976e-05</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0001483508743155112</v>
+        <v>0.0002395779069070804</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0005132559288830433</v>
+        <v>0.0006654967876502115</v>
       </c>
       <c r="M17" t="n">
-        <v>0.007381745700638561</v>
+        <v>0.009388560995797667</v>
       </c>
       <c r="N17" t="n">
-        <v>1.000280198300279</v>
+        <v>1.00045325791973</v>
       </c>
       <c r="O17" t="n">
-        <v>0.007696001897434902</v>
+        <v>0.009788251474389286</v>
       </c>
       <c r="P17" t="n">
-        <v>77.63498049416037</v>
+        <v>76.67305298435831</v>
       </c>
       <c r="Q17" t="n">
-        <v>112.9823794153382</v>
+        <v>112.0204519055361</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_22</t>
+          <t>model_10_1_4</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9999427933725448</v>
+        <v>0.9997354930066573</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9993057822299293</v>
+        <v>0.9990867793559994</v>
       </c>
       <c r="D18" t="n">
-        <v>0.9995138411333958</v>
+        <v>0.999789909882641</v>
       </c>
       <c r="E18" t="n">
-        <v>0.999810741662765</v>
+        <v>0.9996831337690327</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9996312570845128</v>
+        <v>0.9997231183329583</v>
       </c>
       <c r="G18" t="n">
-        <v>5.339987564871437e-05</v>
+        <v>0.0002469056677703143</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0006480218157227568</v>
+        <v>0.0008524513854211045</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0002497428047497179</v>
+        <v>0.0001625958252638908</v>
       </c>
       <c r="J18" t="n">
-        <v>4.8493093200451e-05</v>
+        <v>0.0004106333361372132</v>
       </c>
       <c r="K18" t="n">
-        <v>0.0001491179489750844</v>
+        <v>0.000286614580700552</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0004957957382007694</v>
+        <v>0.001695145030606048</v>
       </c>
       <c r="M18" t="n">
-        <v>0.007307521854138677</v>
+        <v>0.01571323225088696</v>
       </c>
       <c r="N18" t="n">
-        <v>1.000274591811785</v>
+        <v>1.001269633568045</v>
       </c>
       <c r="O18" t="n">
-        <v>0.007618618188124974</v>
+        <v>0.01638217707868213</v>
       </c>
       <c r="P18" t="n">
-        <v>77.6754042813532</v>
+        <v>74.61300841228856</v>
       </c>
       <c r="Q18" t="n">
-        <v>113.022803202531</v>
+        <v>109.9604073334664</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_23</t>
+          <t>model_10_1_21</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9999437329042484</v>
+        <v>0.9999031716746054</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9993030512442316</v>
+        <v>0.999086531714693</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9995135619313553</v>
+        <v>0.9994723384851226</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9998063101110897</v>
+        <v>0.9999240346888946</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9996296758216607</v>
+        <v>0.9997551953387662</v>
       </c>
       <c r="G19" t="n">
-        <v>5.252286404399101e-05</v>
+        <v>9.038499148355098e-05</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0006505710709951123</v>
+        <v>0.0008526825477105742</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0002498862325579425</v>
+        <v>0.0004083750371031464</v>
       </c>
       <c r="J19" t="n">
-        <v>4.962857632659018e-05</v>
+        <v>9.844497797924328e-05</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0001497574044422664</v>
+        <v>0.0002534100075411949</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0004799418552019579</v>
+        <v>0.0006393064197990246</v>
       </c>
       <c r="M19" t="n">
-        <v>0.007247265970280862</v>
+        <v>0.009507102160151167</v>
       </c>
       <c r="N19" t="n">
-        <v>1.000270082059608</v>
+        <v>1.000464775961894</v>
       </c>
       <c r="O19" t="n">
-        <v>0.007555797086544457</v>
+        <v>0.009911839181523351</v>
       </c>
       <c r="P19" t="n">
-        <v>77.70852395514382</v>
+        <v>76.6228646555232</v>
       </c>
       <c r="Q19" t="n">
-        <v>113.0559228763216</v>
+        <v>111.970263576701</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_24</t>
+          <t>model_10_1_22</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.9999444442835511</v>
+        <v>0.999900644436677</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9993005260270135</v>
+        <v>0.9990773849955391</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9995130971825801</v>
+        <v>0.999453556756185</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9998020671105182</v>
+        <v>0.9999153890812866</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9996280364416582</v>
+        <v>0.9997427624626239</v>
       </c>
       <c r="G20" t="n">
-        <v>5.18588226909006e-05</v>
+        <v>9.274405715675431e-05</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0006529282504240374</v>
+        <v>0.0008612206085460879</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0002501249768668836</v>
+        <v>0.0004229108503765336</v>
       </c>
       <c r="J20" t="n">
-        <v>5.071574757180926e-05</v>
+        <v>0.0001096489951575029</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0001504203622193464</v>
+        <v>0.0002662799227670183</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0004657695771103078</v>
+        <v>0.0006156038940205493</v>
       </c>
       <c r="M20" t="n">
-        <v>0.007201307012681837</v>
+        <v>0.009630371600138507</v>
       </c>
       <c r="N20" t="n">
-        <v>1.000266667438955</v>
+        <v>1.00047690670395</v>
       </c>
       <c r="O20" t="n">
-        <v>0.007507881560972283</v>
+        <v>0.01004035645677387</v>
       </c>
       <c r="P20" t="n">
-        <v>77.73397095958191</v>
+        <v>76.57133386462233</v>
       </c>
       <c r="Q20" t="n">
-        <v>113.0813698807597</v>
+        <v>111.9187327858001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_5</t>
+          <t>model_10_1_23</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9997197604937827</v>
+        <v>0.9998979511497862</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9992831694982945</v>
+        <v>0.9990687245164513</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9995435292554453</v>
+        <v>0.9994358610424335</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9998453487034618</v>
+        <v>0.9999068834199331</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9996610771903481</v>
+        <v>0.9997308231676421</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0002615912779612175</v>
+        <v>9.525812224778285e-05</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0006691298081196227</v>
+        <v>0.0008693047856233911</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0002344918335596145</v>
+        <v>0.0004366061598808764</v>
       </c>
       <c r="J21" t="n">
-        <v>3.962583549111833e-05</v>
+        <v>0.0001206716531636568</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0001370588345253664</v>
+        <v>0.0002786389065222666</v>
       </c>
       <c r="L21" t="n">
-        <v>0.001439604751123471</v>
+        <v>0.0005941109987708658</v>
       </c>
       <c r="M21" t="n">
-        <v>0.01617378366249584</v>
+        <v>0.009760026754460402</v>
       </c>
       <c r="N21" t="n">
-        <v>1.001345149629843</v>
+        <v>1.000489834481026</v>
       </c>
       <c r="O21" t="n">
-        <v>0.01686233511735605</v>
+        <v>0.01017553129943842</v>
       </c>
       <c r="P21" t="n">
-        <v>74.49745456012781</v>
+        <v>76.51784054930079</v>
       </c>
       <c r="Q21" t="n">
-        <v>109.8448534813056</v>
+        <v>111.8652394704786</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>model_10_1_4</t>
+          <t>model_10_1_24</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.999670422210583</v>
+        <v>0.9998953433277042</v>
       </c>
       <c r="C22" t="n">
-        <v>0.9992456830468044</v>
+        <v>0.999060679835874</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9995817336135138</v>
+        <v>0.9994200483827894</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9998393904183437</v>
+        <v>0.9998989842249326</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9996834552137248</v>
+        <v>0.9997199674291212</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0003076463996278138</v>
+        <v>9.769240969115246e-05</v>
       </c>
       <c r="H22" t="n">
-        <v>0.000704121765120574</v>
+        <v>0.0008768141418216877</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0002148660194624464</v>
+        <v>0.0004488441103222546</v>
       </c>
       <c r="J22" t="n">
-        <v>4.115250892472803e-05</v>
+        <v>0.000130908379197705</v>
       </c>
       <c r="K22" t="n">
-        <v>0.0001280092641935872</v>
+        <v>0.0002898762447599799</v>
       </c>
       <c r="L22" t="n">
-        <v>0.001552740945132197</v>
+        <v>0.0005745261692225969</v>
       </c>
       <c r="M22" t="n">
-        <v>0.01753985175615272</v>
+        <v>0.009883947070434588</v>
       </c>
       <c r="N22" t="n">
-        <v>1.001581973389202</v>
+        <v>1.00050235202702</v>
       </c>
       <c r="O22" t="n">
-        <v>0.01828655955791069</v>
+        <v>0.01030472715981404</v>
       </c>
       <c r="P22" t="n">
-        <v>74.17311897533</v>
+        <v>76.4673733837821</v>
       </c>
       <c r="Q22" t="n">
-        <v>109.5205178965078</v>
+        <v>111.8147723049599</v>
       </c>
     </row>
     <row r="23">
@@ -1677,52 +1677,52 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9996112599002497</v>
+        <v>0.9996921309561662</v>
       </c>
       <c r="C23" t="n">
-        <v>0.9991956914920596</v>
+        <v>0.999028625245977</v>
       </c>
       <c r="D23" t="n">
-        <v>0.9996245903168337</v>
+        <v>0.9997324146725766</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9998309949536093</v>
+        <v>0.9995994564169708</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9997080160847677</v>
+        <v>0.9996492467347362</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0003628718193987148</v>
+        <v>0.0002873822385297349</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0007507866870992209</v>
+        <v>0.0009067356944566712</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0001928502669488132</v>
+        <v>0.0002070933068525742</v>
       </c>
       <c r="J23" t="n">
-        <v>4.33036535441541e-05</v>
+        <v>0.0005190725034521728</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0001180769602464836</v>
+        <v>0.0003630829051523734</v>
       </c>
       <c r="L23" t="n">
-        <v>0.001676490124379221</v>
+        <v>0.001847423416221687</v>
       </c>
       <c r="M23" t="n">
-        <v>0.01904919471785395</v>
+        <v>0.01695235200583491</v>
       </c>
       <c r="N23" t="n">
-        <v>1.001865952478802</v>
+        <v>1.001477771410402</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0198601583742622</v>
+        <v>0.01767404872692971</v>
       </c>
       <c r="P23" t="n">
-        <v>73.84292180132631</v>
+        <v>74.30939477350384</v>
       </c>
       <c r="Q23" t="n">
-        <v>109.1903207225041</v>
+        <v>109.6567936946817</v>
       </c>
     </row>
     <row r="24">
@@ -1732,52 +1732,52 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9995395263587561</v>
+        <v>0.9996260869073041</v>
       </c>
       <c r="C24" t="n">
-        <v>0.999131615545825</v>
+        <v>0.9989459519016718</v>
       </c>
       <c r="D24" t="n">
-        <v>0.9996662423075011</v>
+        <v>0.9996274855815318</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9998199789646048</v>
+        <v>0.9994913596516323</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9997309815899175</v>
+        <v>0.9995423576197545</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0004298319316444231</v>
+        <v>0.0003490314591437698</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0008105987703002643</v>
+        <v>0.0009839076324251786</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0001714533827464588</v>
+        <v>0.0002883014682220666</v>
       </c>
       <c r="J24" t="n">
-        <v>4.612624719732018e-05</v>
+        <v>0.0006591572806816153</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0001087898149718895</v>
+        <v>0.0004737293744518409</v>
       </c>
       <c r="L24" t="n">
-        <v>0.00181647109080526</v>
+        <v>0.002055797110464237</v>
       </c>
       <c r="M24" t="n">
-        <v>0.02073238846935932</v>
+        <v>0.01868238365797496</v>
       </c>
       <c r="N24" t="n">
-        <v>1.002210273477971</v>
+        <v>1.00179478284494</v>
       </c>
       <c r="O24" t="n">
-        <v>0.02161500916846055</v>
+        <v>0.01947773140816059</v>
       </c>
       <c r="P24" t="n">
-        <v>73.50423256464381</v>
+        <v>73.92069699802238</v>
       </c>
       <c r="Q24" t="n">
-        <v>108.8516314858216</v>
+        <v>109.2680959192002</v>
       </c>
     </row>
     <row r="25">
@@ -1787,52 +1787,52 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9994512603032532</v>
+        <v>0.9995316351734224</v>
       </c>
       <c r="C25" t="n">
-        <v>0.9990511905463527</v>
+        <v>0.9988317104238882</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9997015219726079</v>
+        <v>0.9994538710055684</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9998059724841178</v>
+        <v>0.9993518553402101</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9997489522963642</v>
+        <v>0.9993901323151445</v>
       </c>
       <c r="G25" t="n">
-        <v>0.0005122244200242855</v>
+        <v>0.0004371980067703722</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0008856719770581218</v>
+        <v>0.001090547037314931</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0001533300014412048</v>
+        <v>0.0004226676421833509</v>
       </c>
       <c r="J25" t="n">
-        <v>4.971508546775669e-05</v>
+        <v>0.0008399437299978526</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0001015225434544808</v>
+        <v>0.0006313056860906018</v>
       </c>
       <c r="L25" t="n">
-        <v>0.001972265720856518</v>
+        <v>0.002327378717756163</v>
       </c>
       <c r="M25" t="n">
-        <v>0.02263237548345921</v>
+        <v>0.02090928039819573</v>
       </c>
       <c r="N25" t="n">
-        <v>1.002633950544385</v>
+        <v>1.002248151167573</v>
       </c>
       <c r="O25" t="n">
-        <v>0.02359588256326601</v>
+        <v>0.02179943175292431</v>
       </c>
       <c r="P25" t="n">
-        <v>73.15349541719829</v>
+        <v>73.47024872150389</v>
       </c>
       <c r="Q25" t="n">
-        <v>108.5008943383761</v>
+        <v>108.8176476426817</v>
       </c>
     </row>
     <row r="26">
@@ -1842,52 +1842,52 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.9993415916155013</v>
+        <v>0.9993927197963429</v>
       </c>
       <c r="C26" t="n">
-        <v>0.9989506508769683</v>
+        <v>0.9986724312678104</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9997274666037166</v>
+        <v>0.9991841865626578</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9997869203752489</v>
+        <v>0.9991529998511214</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9997593953575812</v>
+        <v>0.9991648423239521</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0006145953261416769</v>
+        <v>0.0005668694135937132</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0009795213452470086</v>
+        <v>0.001239227137966608</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0001400020846091241</v>
+        <v>0.0006313855252856595</v>
       </c>
       <c r="J26" t="n">
-        <v>5.459674988764891e-05</v>
+        <v>0.001097644566860308</v>
       </c>
       <c r="K26" t="n">
-        <v>9.729941724838649e-05</v>
+        <v>0.0008645150460729838</v>
       </c>
       <c r="L26" t="n">
-        <v>0.002143735861123751</v>
+        <v>0.002652333646150909</v>
       </c>
       <c r="M26" t="n">
-        <v>0.02479103318019798</v>
+        <v>0.02380901958489079</v>
       </c>
       <c r="N26" t="n">
-        <v>1.003160360245594</v>
+        <v>1.002914944977554</v>
       </c>
       <c r="O26" t="n">
-        <v>0.0258464387871924</v>
+        <v>0.0248226188400846</v>
       </c>
       <c r="P26" t="n">
-        <v>72.78909302602518</v>
+        <v>72.9507631837688</v>
       </c>
       <c r="Q26" t="n">
-        <v>108.136491947203</v>
+        <v>108.2981621049466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>